<commit_message>
install virtualbox on macos
</commit_message>
<xml_diff>
--- a/miniOS/miniOS.xlsx
+++ b/miniOS/miniOS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BC013D-552D-4A9B-97B3-DFD9F4276CB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A099831-5607-429E-941F-A8FCC45113D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="run first" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>first.s</t>
   </si>
@@ -62,22 +62,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">on </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mac OS</t>
-    </r>
-  </si>
-  <si>
     <t>can be installed</t>
   </si>
   <si>
@@ -85,9 +69,6 @@
   </si>
   <si>
     <t>step 1</t>
-  </si>
-  <si>
-    <t>install a hypervisor on Windows or MacOS</t>
   </si>
   <si>
     <r>
@@ -121,12 +102,77 @@
   <si>
     <t>Ubuntu Desktop</t>
   </si>
+  <si>
+    <t>Hypervisor</t>
+  </si>
+  <si>
+    <t>Physical machine</t>
+  </si>
+  <si>
+    <t>Virtual Machine(s)</t>
+  </si>
+  <si>
+    <t>step 3</t>
+  </si>
+  <si>
+    <t>GNU assembler (GAS)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">install </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GNU assembler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on Ubuntu</t>
+    </r>
+  </si>
+  <si>
+    <t>### 02 GNU assembler, Linux Desktop, virtual machine &amp; hypervisor</t>
+  </si>
+  <si>
+    <t>macOS or Windows</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">on </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>macOS</t>
+    </r>
+  </si>
+  <si>
+    <t>install a hypervisor on Windows or macOS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,16 +217,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -188,16 +246,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:K17"/>
+  <dimension ref="C2:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,12 +776,17 @@
     <col min="7" max="7" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.35">
       <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.35">
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
@@ -565,59 +799,118 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.35">
       <c r="I7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.35">
       <c r="I9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="E13" t="s">
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="F14" t="s">
+      <c r="F24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="E16" t="s">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F17" s="3" t="s">
-        <v>15</v>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>